<commit_message>
added recommendations to export
</commit_message>
<xml_diff>
--- a/app/src/main/assets/report_rmi_v2.xlsx
+++ b/app/src/main/assets/report_rmi_v2.xlsx
@@ -12,30 +12,48 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjM+4RVD1qvMndAJgB48jLLT8jRaA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhTUx0R/p8nmpr8ODFtPV++3D6Sjw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="257">
+  <si>
+    <t>SCHOOL ACCREDITATION STATUS REPORT – FORM B</t>
+  </si>
   <si>
     <t>Summary of School Evaluation Scores</t>
   </si>
   <si>
-    <t>SCHOOL ACCREDITATION STATUS REPORT – FORM B</t>
+    <t>Note this is a preview of the FORM B only. The results are not final and official until verified and signed by the SDOE Director and the NDOE Secretary</t>
+  </si>
+  <si>
+    <t>$schNo</t>
+  </si>
+  <si>
+    <t>$schName</t>
   </si>
   <si>
     <t>Summary of Classroom Observation 1 Scores</t>
   </si>
   <si>
+    <t>$date</t>
+  </si>
+  <si>
+    <t>$principal</t>
+  </si>
+  <si>
     <t>Summary of Classroom Observation 2 Scores</t>
   </si>
   <si>
     <t>School Number</t>
   </si>
   <si>
+    <t>Summary of School Evaluation/Classroom Observation Scores</t>
+  </si>
+  <si>
     <t>School Name</t>
   </si>
   <si>
@@ -45,30 +63,15 @@
     <t>Standard 1</t>
   </si>
   <si>
-    <t>Note this is a preview of the FORM B only. The results are not final and official until verified and signed by the SDOE Director and the NDOE Secretary</t>
-  </si>
-  <si>
-    <t>$schNo</t>
-  </si>
-  <si>
     <t>Standard 2</t>
   </si>
   <si>
-    <t>$schName</t>
-  </si>
-  <si>
-    <t>$date</t>
-  </si>
-  <si>
-    <t>$principal</t>
+    <t>School Evaluation</t>
   </si>
   <si>
     <t>Standard 3</t>
   </si>
   <si>
-    <t>Summary of School Evaluation/Classroom Observation Scores</t>
-  </si>
-  <si>
     <t>Standard 4</t>
   </si>
   <si>
@@ -78,18 +81,15 @@
     <t>Standard 6</t>
   </si>
   <si>
-    <t>School Evaluation</t>
-  </si>
-  <si>
     <t>Classroom Observation 1</t>
   </si>
   <si>
+    <t>Classroom Observation 2</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
-    <t>Classroom Observation 2</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -784,6 +784,12 @@
   </si>
   <si>
     <t>$tallyLevel</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
+  </si>
+  <si>
+    <t>$recommendations</t>
   </si>
 </sst>
 </file>
@@ -797,20 +803,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="11.0"/>
+      <sz val="18.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <b/>
+      <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -819,14 +818,9 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -837,6 +831,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -853,11 +859,14 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="18.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -898,7 +907,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border/>
     <border>
       <left/>
@@ -949,6 +958,13 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -958,18 +974,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -988,6 +992,12 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right/>
       <top/>
       <bottom/>
     </border>
@@ -995,9 +1005,8 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -1042,113 +1051,116 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="9" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="14" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1157,38 +1169,41 @@
     <xf borderId="14" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="19" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1420,172 +1435,172 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="6" t="s">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="11" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="6" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="11" t="s">
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="14" t="s">
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="16" t="s">
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="AN2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="14" t="s">
+      <c r="AM2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="16" t="s">
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="17" t="s">
         <v>17</v>
+      </c>
+      <c r="AY2" s="18" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="A3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="26" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="27" t="s">
@@ -1600,16 +1615,16 @@
       <c r="K3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="26" t="s">
         <v>26</v>
       </c>
       <c r="P3" s="27" t="s">
@@ -1624,16 +1639,16 @@
       <c r="S3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="V3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="W3" s="26" t="s">
         <v>26</v>
       </c>
       <c r="X3" s="27" t="s">
@@ -1648,10 +1663,10 @@
       <c r="AA3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="AB3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AC3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="AD3" s="27" t="s">
@@ -1666,28 +1681,28 @@
       <c r="AG3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AH3" s="32" t="s">
+      <c r="AH3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AI3" s="32" t="s">
+      <c r="AI3" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AJ3" s="32" t="s">
+      <c r="AJ3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AK3" s="32" t="s">
+      <c r="AK3" s="29" t="s">
         <v>26</v>
       </c>
       <c r="AL3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="25" t="s">
+      <c r="AM3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AN3" s="25" t="s">
+      <c r="AN3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="AO3" s="25" t="s">
+      <c r="AO3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="AP3" s="27" t="s">
@@ -1702,22 +1717,22 @@
       <c r="AS3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AT3" s="32" t="s">
+      <c r="AT3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="32" t="s">
+      <c r="AU3" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AV3" s="32" t="s">
+      <c r="AV3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AW3" s="32" t="s">
+      <c r="AW3" s="29" t="s">
         <v>26</v>
       </c>
       <c r="AX3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AY3" s="25" t="s">
+      <c r="AY3" s="26" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2705,6 +2720,13 @@
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="AB1:AM1"/>
+    <mergeCell ref="D1:AA1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="T2:W2"/>
     <mergeCell ref="AN1:AY1"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -2712,13 +2734,6 @@
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="D1:AA1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="T2:W2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2741,224 +2756,224 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>8</v>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>11</v>
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>13</v>
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12"/>
+      <c r="A5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="3"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AW6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="18" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AW7" s="3"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
-      <c r="B8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="21" t="s">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="26" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="21" t="s">
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="26" t="s">
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="24"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="22"/>
       <c r="Z8" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="22"/>
-      <c r="AI8" s="24"/>
-      <c r="AJ8" s="31" t="s">
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="31" t="s">
         <v>16</v>
       </c>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="22"/>
+      <c r="AJ8" s="32" t="s">
+        <v>17</v>
+      </c>
       <c r="AK8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM8" s="22"/>
+      <c r="AN8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="22"/>
+      <c r="AR8" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="22"/>
+      <c r="AV8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="AL8" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="AO8" s="22"/>
-      <c r="AP8" s="22"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="AS8" s="22"/>
-      <c r="AT8" s="22"/>
-      <c r="AU8" s="24"/>
-      <c r="AV8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW8" s="31" t="s">
-        <v>17</v>
+      <c r="AW8" s="32" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -3117,16 +3132,16 @@
       <c r="AI10" s="33">
         <v>4.0</v>
       </c>
-      <c r="AJ10" s="31">
+      <c r="AJ10" s="32">
         <v>1.0</v>
       </c>
       <c r="AK10" s="33">
         <v>1.0</v>
       </c>
-      <c r="AL10" s="31">
+      <c r="AL10" s="32">
         <v>1.0</v>
       </c>
-      <c r="AM10" s="31">
+      <c r="AM10" s="32">
         <v>2.0</v>
       </c>
       <c r="AN10" s="33">
@@ -3141,22 +3156,22 @@
       <c r="AQ10" s="33">
         <v>4.0</v>
       </c>
-      <c r="AR10" s="31">
+      <c r="AR10" s="32">
         <v>1.0</v>
       </c>
-      <c r="AS10" s="31">
+      <c r="AS10" s="32">
         <v>2.0</v>
       </c>
-      <c r="AT10" s="31">
+      <c r="AT10" s="32">
         <v>3.0</v>
       </c>
-      <c r="AU10" s="31">
+      <c r="AU10" s="32">
         <v>4.0</v>
       </c>
       <c r="AV10" s="33">
         <v>1.0</v>
       </c>
-      <c r="AW10" s="31">
+      <c r="AW10" s="32">
         <v>1.0</v>
       </c>
     </row>
@@ -4111,56 +4126,66 @@
       <c r="A19" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20">
-      <c r="A20" s="52">
+      <c r="A20" s="50">
         <v>1.0</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="50">
         <v>2.0</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C20" s="50">
         <v>3.0</v>
       </c>
-      <c r="D20" s="52">
+      <c r="D20" s="50">
         <v>4.0</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="50" t="s">
         <v>247</v>
       </c>
-      <c r="F20" s="52" t="s">
+      <c r="F20" s="50" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="52" t="s">
         <v>251</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="52" t="s">
         <v>252</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="52" t="s">
         <v>253</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="53" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="23" ht="21.0" customHeight="1">
+      <c r="A23" s="54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="55"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="55" t="s">
+        <v>256</v>
+      </c>
+    </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>
@@ -5136,78 +5161,79 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="AR10:AR11"/>
+    <mergeCell ref="AS10:AS11"/>
+    <mergeCell ref="AF10:AF11"/>
+    <mergeCell ref="AE10:AE11"/>
+    <mergeCell ref="AD10:AD11"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AN10:AN11"/>
+    <mergeCell ref="AO10:AO11"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AI10:AI11"/>
+    <mergeCell ref="AH10:AH11"/>
+    <mergeCell ref="AC10:AC11"/>
+    <mergeCell ref="AP10:AP11"/>
+    <mergeCell ref="AU10:AU11"/>
+    <mergeCell ref="AT10:AT11"/>
+    <mergeCell ref="AQ10:AQ11"/>
+    <mergeCell ref="AV10:AV11"/>
+    <mergeCell ref="AW10:AW11"/>
+    <mergeCell ref="B7:Y7"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="R8:U9"/>
+    <mergeCell ref="F8:I9"/>
+    <mergeCell ref="B8:E9"/>
+    <mergeCell ref="J8:M9"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="V8:Y9"/>
+    <mergeCell ref="AF8:AI9"/>
+    <mergeCell ref="AL7:AW7"/>
+    <mergeCell ref="Z7:AK7"/>
+    <mergeCell ref="AB8:AE9"/>
+    <mergeCell ref="Z8:AA9"/>
+    <mergeCell ref="A6:AW6"/>
+    <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="R10:R11"/>
-    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="AJ8:AJ9"/>
+    <mergeCell ref="AR8:AU9"/>
+    <mergeCell ref="AN8:AQ9"/>
+    <mergeCell ref="AK8:AK9"/>
+    <mergeCell ref="AL8:AM9"/>
+    <mergeCell ref="AW8:AW9"/>
+    <mergeCell ref="AV8:AV9"/>
     <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="N10:N11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="AA10:AA11"/>
     <mergeCell ref="L10:L11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="V8:Y9"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="AC10:AC11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="AV10:AV11"/>
-    <mergeCell ref="AW10:AW11"/>
-    <mergeCell ref="AJ8:AJ9"/>
-    <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="AL8:AM9"/>
-    <mergeCell ref="F8:I9"/>
-    <mergeCell ref="B8:E9"/>
-    <mergeCell ref="AF10:AF11"/>
-    <mergeCell ref="AE10:AE11"/>
-    <mergeCell ref="AP10:AP11"/>
-    <mergeCell ref="AQ10:AQ11"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="AH10:AH11"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="AI10:AI11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="J8:M9"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="A6:AW6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="AL7:AW7"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AN10:AN11"/>
-    <mergeCell ref="AO10:AO11"/>
-    <mergeCell ref="AW8:AW9"/>
-    <mergeCell ref="AV8:AV9"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AF8:AI9"/>
-    <mergeCell ref="AB8:AE9"/>
-    <mergeCell ref="B7:Y7"/>
-    <mergeCell ref="Z7:AK7"/>
-    <mergeCell ref="AU10:AU11"/>
-    <mergeCell ref="AT10:AT11"/>
-    <mergeCell ref="R8:U9"/>
-    <mergeCell ref="Z8:AA9"/>
-    <mergeCell ref="AD10:AD11"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AR8:AU9"/>
-    <mergeCell ref="AN8:AQ9"/>
-    <mergeCell ref="AR10:AR11"/>
-    <mergeCell ref="AS10:AS11"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>